<commit_message>
fixed the planning to remove extra userstories that were not planned
</commit_message>
<xml_diff>
--- a/Sprint Backlog/Sprint1/Planning and Burndown/Initial Planning and Burndown Chart.xlsx
+++ b/Sprint Backlog/Sprint1/Planning and Burndown/Initial Planning and Burndown Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\Team27\Team27\Sprint1\Planning and Burndown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\Team27\Team27\Sprint Backlog\Sprint1\Planning and Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A21996-A9DF-4859-A115-F079F8F03E27}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F7FBA6-E515-4384-B8D7-5C897473BF22}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" xr2:uid="{E26ED3F2-7FF5-461C-B9EE-AAC597F16CF8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>User Stories</t>
   </si>
@@ -122,9 +122,6 @@
     <t>18</t>
   </si>
   <si>
-    <t>T:1</t>
-  </si>
-  <si>
     <t>T:2</t>
   </si>
   <si>
@@ -158,42 +155,9 @@
     <t>28</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>A:3</t>
   </si>
   <si>
-    <t>T:4</t>
-  </si>
-  <si>
-    <t>V:2</t>
-  </si>
-  <si>
-    <t>V:3</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -237,24 +201,6 @@
   </si>
   <si>
     <t>Planned to finish</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>T33</t>
   </si>
   <si>
     <t>A  = ARNOB (Talukder)</t>
@@ -285,18 +231,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -348,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -357,14 +297,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -373,8 +320,42 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -395,17 +376,15 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
+        <right/>
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
@@ -413,10 +392,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -437,9 +412,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -453,10 +428,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -477,49 +448,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -552,9 +483,9 @@
         <scheme val="minor"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -567,10 +498,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -591,9 +518,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -607,10 +534,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -631,9 +554,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -647,10 +570,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -671,9 +590,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -687,10 +606,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -711,9 +626,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -727,10 +642,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -751,9 +662,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -767,10 +678,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -791,9 +698,9 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -809,6 +716,61 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -845,9 +807,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1997,20 +1956,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B31CD5ED-DA30-4B5B-9C2E-BD07FBAC5C04}" name="Table1" displayName="Table1" ref="A1:K35" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A1:K34" xr:uid="{4F9759AE-BCDD-4C93-BCA3-CA94BFA349CB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B31CD5ED-DA30-4B5B-9C2E-BD07FBAC5C04}" name="Table1" displayName="Table1" ref="A1:K22" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24" totalsRowDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A1:K21" xr:uid="{4F9759AE-BCDD-4C93-BCA3-CA94BFA349CB}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{3ACA0BEF-0DA9-435F-A244-9672369B292D}" name="User Stories" dataDxfId="19" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{6DF7373E-780B-4E1C-BCF0-8615D6B337E5}" name="Tasks" dataDxfId="17" totalsRowDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{D38495B2-E249-445F-8D51-8F668993E4A3}" name="Dependency" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{D1964B85-D35A-4849-B42D-0A0B7B68C7CD}" name="Story Points" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{D0DD318F-1642-444A-A573-1CB8CE779AA1}" name="1" dataDxfId="11" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{E11F2DB4-BF31-48F4-9587-DD065D2831E2}" name="2" dataDxfId="9" totalsRowDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{FA4A994B-7981-4C59-983E-DB99A0267023}" name="3" totalsRowDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{B24FEE48-3B4F-4046-8BAE-3ED79A683D7A}" name="4" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{12163C1F-33DD-4916-9BD4-F716888134BC}" name="5" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{D01478F4-27AB-4127-84CE-DE02C992490D}" name="6" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{2AF698B0-89D9-4053-8508-224FD96C396F}" name="7" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3ACA0BEF-0DA9-435F-A244-9672369B292D}" name="User Stories" dataDxfId="21" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{6DF7373E-780B-4E1C-BCF0-8615D6B337E5}" name="Tasks" dataDxfId="20" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{D38495B2-E249-445F-8D51-8F668993E4A3}" name="Dependency" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{D1964B85-D35A-4849-B42D-0A0B7B68C7CD}" name="Story Points" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{D0DD318F-1642-444A-A573-1CB8CE779AA1}" name="1" dataDxfId="19" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{E11F2DB4-BF31-48F4-9587-DD065D2831E2}" name="2" dataDxfId="18" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{FA4A994B-7981-4C59-983E-DB99A0267023}" name="3" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{B24FEE48-3B4F-4046-8BAE-3ED79A683D7A}" name="4" dataDxfId="17" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{12163C1F-33DD-4916-9BD4-F716888134BC}" name="5" dataDxfId="16" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{D01478F4-27AB-4127-84CE-DE02C992490D}" name="6" dataDxfId="15" totalsRowDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{2AF698B0-89D9-4053-8508-224FD96C396F}" name="7" dataDxfId="14" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2020,7 +1979,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{05D8F1E3-0789-4F1C-A68C-AC72022968A7}" name="burndown" displayName="burndown" ref="A1:I5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I5" xr:uid="{B0649E73-B99F-4382-B739-27E9FADA64DE}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{BEAED5CF-41A6-49A4-8D73-CE3EE0BE9EC2}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{BEAED5CF-41A6-49A4-8D73-CE3EE0BE9EC2}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{F65FF7AC-9761-4A5B-95A1-A36B3EEC1F3A}" uniqueName="2" name="Column2" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{B57E2A10-2BF4-40E9-91E2-D5DACF4797C0}" uniqueName="3" name="Column3" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{F9713ACA-8B31-4E95-B3DB-ECB502813E2B}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
@@ -2331,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FDF196-0978-4E31-AD1C-547BFF446FB7}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,7 +2339,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2403,7 +2362,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2426,7 +2385,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2450,7 +2409,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2474,7 +2433,7 @@
       <c r="I5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2489,7 +2448,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2"/>
       <c r="H6" s="2"/>
@@ -2530,7 +2489,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -2550,7 +2509,7 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2569,7 +2528,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2604,7 +2563,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
@@ -2624,7 +2583,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2">
@@ -2644,7 +2603,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2">
@@ -2663,7 +2622,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2">
@@ -2683,7 +2642,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2">
@@ -2702,7 +2661,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
@@ -2722,7 +2681,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2">
@@ -2740,7 +2699,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2">
@@ -2760,7 +2719,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -2780,7 +2739,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2">
@@ -2796,278 +2755,219 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>8</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="I22" t="s">
-        <v>47</v>
-      </c>
-      <c r="J22" t="s">
-        <v>26</v>
-      </c>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="8">
+        <f>SUBTOTAL(109,Table1[Story Points])</f>
+        <v>56</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>8</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2">
-        <v>5</v>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="3">
+        <v>56</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>8</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>8</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2">
-        <v>5</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>9</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2">
-        <v>3</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>9</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>9</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="2">
-        <v>2</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>9</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="2">
-        <v>3</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>9</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="3">
-        <v>3</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>9</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="3">
-        <v>3</v>
-      </c>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>9</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3</v>
-      </c>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>9</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="3">
-        <v>4</v>
-      </c>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>9</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" s="2">
-        <v>5</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="5">
-        <f>SUBTOTAL(109,Table1[Story Points])</f>
-        <v>103</v>
-      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="6"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="6"/>
+      <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="7"/>
+      <c r="K35" s="5"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="3">
-        <v>56</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3092,36 +2992,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>56</v>
@@ -3129,7 +3029,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3158,7 +3058,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>56</v>
@@ -3187,7 +3087,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>56</v>

</xml_diff>